<commit_message>
Lots of detailed schema updates; updated model diagram
</commit_message>
<xml_diff>
--- a/repository/isa_immport/InvestigationSchemaControlledTerms.xlsx
+++ b/repository/isa_immport/InvestigationSchemaControlledTerms.xlsx
@@ -1113,13 +1113,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="3" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" customWidth="1"/>
     <col min="4" max="4" width="28.1640625" customWidth="1"/>
     <col min="5" max="5" width="55.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.6640625" bestFit="1" customWidth="1"/>

</xml_diff>